<commit_message>
Oregon data cleaning up - filter, mutate to combine 3 categories into complete_or_not_eligible
</commit_message>
<xml_diff>
--- a/Data/ODE data.xlsx
+++ b/Data/ODE data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hata/Desktop/EDLD652_Diss/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE3EB65A-081F-BF43-92B3-250802790E26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A7E7E60-A909-024A-8943-D5FF071B8CC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6020" yWindow="500" windowWidth="20580" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="180" yWindow="500" windowWidth="22780" windowHeight="12200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -231,7 +231,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -264,6 +264,24 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -479,10 +497,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P992"/>
+  <dimension ref="A1:P991"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37:XFD38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A46" sqref="A46:XFD46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -573,7 +593,7 @@
         <v>0</v>
       </c>
       <c r="M2" s="6">
-        <f t="shared" ref="M2:M8" si="0">SUM(D2:L2)</f>
+        <f>SUM(D2:L2)</f>
         <v>2</v>
       </c>
       <c r="P2" s="7">
@@ -583,61 +603,61 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B3" s="5">
-        <v>1290</v>
+        <v>860</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D3" s="6">
-        <v>138</v>
+        <v>0</v>
       </c>
       <c r="E3" s="6">
-        <v>1678</v>
+        <v>4</v>
       </c>
       <c r="F3" s="6">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="G3" s="6">
-        <v>190</v>
+        <v>0</v>
       </c>
       <c r="H3" s="6">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="I3" s="6">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="J3" s="6">
-        <v>154</v>
+        <v>0</v>
       </c>
       <c r="K3" s="6">
-        <v>464</v>
+        <v>0</v>
       </c>
       <c r="L3" s="6">
-        <v>229</v>
+        <v>0</v>
       </c>
       <c r="M3" s="6">
-        <f t="shared" si="0"/>
-        <v>2900</v>
+        <f>SUM(D3:L3)</f>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B4" s="5">
-        <v>3830</v>
+        <v>860</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D4" s="6">
         <v>0</v>
       </c>
       <c r="E4" s="6">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F4" s="6">
         <v>0</v>
@@ -652,40 +672,40 @@
         <v>0</v>
       </c>
       <c r="J4" s="6">
+        <v>0</v>
+      </c>
+      <c r="K4" s="6">
+        <v>0</v>
+      </c>
+      <c r="L4" s="6">
         <v>1</v>
       </c>
-      <c r="K4" s="6">
-        <v>1</v>
-      </c>
-      <c r="L4" s="6">
-        <v>0</v>
-      </c>
       <c r="M4" s="6">
-        <f t="shared" si="0"/>
-        <v>9</v>
+        <f>SUM(D4:L4)</f>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B5" s="5">
-        <v>4050</v>
+        <v>860</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D5" s="6">
         <v>0</v>
       </c>
       <c r="E5" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5" s="6">
         <v>0</v>
       </c>
       <c r="G5" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H5" s="6">
         <v>0</v>
@@ -703,50 +723,50 @@
         <v>0</v>
       </c>
       <c r="M5" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>SUM(D5:L5)</f>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B6" s="5">
-        <v>4260</v>
+        <v>860</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D6" s="6">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="E6" s="6">
-        <v>250</v>
+        <v>2</v>
       </c>
       <c r="F6" s="6">
+        <v>0</v>
+      </c>
+      <c r="G6" s="6">
         <v>1</v>
       </c>
-      <c r="G6" s="6">
-        <v>33</v>
-      </c>
       <c r="H6" s="6">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I6" s="6">
         <v>0</v>
       </c>
       <c r="J6" s="6">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="K6" s="6">
-        <v>62</v>
+        <v>1</v>
       </c>
       <c r="L6" s="6">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="M6" s="6">
-        <f t="shared" si="0"/>
-        <v>414</v>
+        <f>SUM(D6:L6)</f>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
@@ -754,257 +774,251 @@
         <v>13</v>
       </c>
       <c r="B7" s="5">
-        <v>4800</v>
+        <v>1290</v>
       </c>
       <c r="C7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="6">
+        <v>138</v>
+      </c>
+      <c r="E7" s="6">
+        <v>1678</v>
+      </c>
+      <c r="F7" s="6">
         <v>19</v>
       </c>
-      <c r="D7" s="6">
-        <v>0</v>
-      </c>
-      <c r="E7" s="6">
-        <v>4</v>
-      </c>
-      <c r="F7" s="6">
-        <v>0</v>
-      </c>
       <c r="G7" s="6">
-        <v>0</v>
+        <v>190</v>
       </c>
       <c r="H7" s="6">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="I7" s="6">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="J7" s="6">
-        <v>0</v>
+        <v>154</v>
       </c>
       <c r="K7" s="6">
-        <v>2</v>
+        <v>464</v>
       </c>
       <c r="L7" s="6">
-        <v>2</v>
+        <v>229</v>
       </c>
       <c r="M7" s="6">
-        <f t="shared" si="0"/>
-        <v>8</v>
+        <f>SUM(D7:L7)</f>
+        <v>2900</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B8" s="9">
-        <v>9999</v>
+        <v>1290</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D8" s="10">
-        <v>8</v>
+        <v>111</v>
       </c>
       <c r="E8" s="10">
-        <v>247</v>
+        <v>1714</v>
       </c>
       <c r="F8" s="10">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="G8" s="10">
-        <v>23</v>
+        <v>154</v>
       </c>
       <c r="H8" s="10">
-        <v>5</v>
+        <v>58</v>
       </c>
       <c r="I8" s="10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J8" s="10">
-        <v>38</v>
+        <v>129</v>
       </c>
       <c r="K8" s="10">
-        <v>74</v>
+        <v>571</v>
       </c>
       <c r="L8" s="10">
-        <v>22</v>
+        <v>242</v>
       </c>
       <c r="M8" s="10">
-        <f t="shared" si="0"/>
-        <v>426</v>
+        <f>SUM(D8:L8)</f>
+        <v>3007</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11" t="s">
-        <v>12</v>
+        <v>22</v>
+      </c>
+      <c r="B9" s="14">
+        <v>1290</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>15</v>
       </c>
       <c r="D9" s="12">
-        <f t="shared" ref="D9:M9" si="1">SUM(D2:D8)</f>
-        <v>159</v>
+        <v>123</v>
       </c>
       <c r="E9" s="12">
-        <f t="shared" si="1"/>
-        <v>2187</v>
+        <v>1220</v>
       </c>
       <c r="F9" s="12">
-        <f t="shared" si="1"/>
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="G9" s="12">
-        <f t="shared" si="1"/>
-        <v>246</v>
+        <v>103</v>
       </c>
       <c r="H9" s="12">
-        <f t="shared" si="1"/>
-        <v>29</v>
+        <v>56</v>
       </c>
       <c r="I9" s="12">
-        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="J9" s="12">
+        <v>130</v>
+      </c>
+      <c r="K9" s="12">
+        <v>491</v>
+      </c>
+      <c r="L9" s="12">
+        <v>262</v>
+      </c>
+      <c r="M9" s="12">
+        <f>SUM(D9:L9)</f>
+        <v>2418</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="5">
+        <v>1290</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="6">
+        <v>104</v>
+      </c>
+      <c r="E10" s="6">
+        <v>1409</v>
+      </c>
+      <c r="F10" s="6">
+        <v>16</v>
+      </c>
+      <c r="G10" s="6">
+        <v>116</v>
+      </c>
+      <c r="H10" s="6">
+        <v>10</v>
+      </c>
+      <c r="I10" s="6">
         <v>8</v>
       </c>
-      <c r="J9" s="12">
-        <f t="shared" si="1"/>
-        <v>205</v>
-      </c>
-      <c r="K9" s="12">
-        <f t="shared" si="1"/>
-        <v>604</v>
-      </c>
-      <c r="L9" s="12">
-        <f t="shared" si="1"/>
-        <v>293</v>
-      </c>
-      <c r="M9" s="12">
-        <f t="shared" si="1"/>
-        <v>3759</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" ht="85" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K10" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="L10" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="M10" s="3" t="s">
-        <v>12</v>
+      <c r="J10" s="6">
+        <v>156</v>
+      </c>
+      <c r="K10" s="6">
+        <v>482</v>
+      </c>
+      <c r="L10" s="6">
+        <v>219</v>
+      </c>
+      <c r="M10" s="6">
+        <f>SUM(D10:L10)</f>
+        <v>2520</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B11" s="5">
-        <v>860</v>
+        <v>1290</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D11" s="6">
-        <v>0</v>
+        <v>97</v>
       </c>
       <c r="E11" s="6">
-        <v>4</v>
+        <v>1597</v>
       </c>
       <c r="F11" s="6">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G11" s="6">
-        <v>0</v>
+        <v>123</v>
       </c>
       <c r="H11" s="6">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="I11" s="6">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="J11" s="6">
-        <v>0</v>
+        <v>149</v>
       </c>
       <c r="K11" s="6">
-        <v>0</v>
+        <v>489</v>
       </c>
       <c r="L11" s="6">
-        <v>0</v>
+        <v>187</v>
       </c>
       <c r="M11" s="6">
-        <f t="shared" ref="M11:M17" si="2">SUM(D11:L11)</f>
-        <v>4</v>
+        <f>SUM(D11:L11)</f>
+        <v>2680</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B12" s="5">
-        <v>1290</v>
+        <v>9999</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D12" s="6">
-        <v>111</v>
+        <v>8</v>
       </c>
       <c r="E12" s="6">
-        <v>1714</v>
+        <v>247</v>
       </c>
       <c r="F12" s="6">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="G12" s="6">
-        <v>154</v>
+        <v>23</v>
       </c>
       <c r="H12" s="6">
-        <v>58</v>
+        <v>5</v>
       </c>
       <c r="I12" s="6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J12" s="6">
-        <v>129</v>
+        <v>38</v>
       </c>
       <c r="K12" s="6">
-        <v>571</v>
+        <v>74</v>
       </c>
       <c r="L12" s="6">
-        <v>242</v>
+        <v>22</v>
       </c>
       <c r="M12" s="6">
-        <f t="shared" si="2"/>
-        <v>3007</v>
+        <f>SUM(D12:L12)</f>
+        <v>426</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
@@ -1012,41 +1026,41 @@
         <v>21</v>
       </c>
       <c r="B13" s="5">
-        <v>3830</v>
+        <v>9999</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D13" s="6">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="E13" s="6">
+        <v>266</v>
+      </c>
+      <c r="F13" s="6">
+        <v>8</v>
+      </c>
+      <c r="G13" s="6">
+        <v>17</v>
+      </c>
+      <c r="H13" s="6">
+        <v>11</v>
+      </c>
+      <c r="I13" s="6">
         <v>1</v>
       </c>
-      <c r="F13" s="6">
-        <v>0</v>
-      </c>
-      <c r="G13" s="6">
-        <v>0</v>
-      </c>
-      <c r="H13" s="6">
-        <v>0</v>
-      </c>
-      <c r="I13" s="6">
-        <v>0</v>
-      </c>
       <c r="J13" s="6">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="K13" s="6">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="L13" s="6">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="M13" s="6">
-        <f t="shared" si="2"/>
-        <v>5</v>
+        <f>SUM(D13:L13)</f>
+        <v>475</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
@@ -1054,216 +1068,207 @@
         <v>21</v>
       </c>
       <c r="B14" s="5">
-        <v>4050</v>
+        <v>9999</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D14" s="6">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E14" s="6">
-        <v>0</v>
+        <v>171</v>
       </c>
       <c r="F14" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14" s="6">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="H14" s="6">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I14" s="6">
         <v>0</v>
       </c>
       <c r="J14" s="6">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="K14" s="6">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="L14" s="6">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="M14" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>SUM(D14:L14)</f>
+        <v>342</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B15" s="5">
-        <v>4260</v>
+        <v>9999</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D15" s="6">
+        <v>11</v>
+      </c>
+      <c r="E15" s="6">
+        <v>259</v>
+      </c>
+      <c r="F15" s="6">
+        <v>1</v>
+      </c>
+      <c r="G15" s="6">
+        <v>14</v>
+      </c>
+      <c r="H15" s="6">
         <v>6</v>
       </c>
-      <c r="E15" s="6">
-        <v>244</v>
-      </c>
-      <c r="F15" s="6">
-        <v>3</v>
-      </c>
-      <c r="G15" s="6">
-        <v>21</v>
-      </c>
-      <c r="H15" s="6">
-        <v>7</v>
-      </c>
       <c r="I15" s="6">
         <v>0</v>
       </c>
       <c r="J15" s="6">
-        <v>5</v>
+        <v>45</v>
       </c>
       <c r="K15" s="6">
-        <v>47</v>
+        <v>98</v>
       </c>
       <c r="L15" s="6">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="M15" s="6">
-        <f t="shared" si="2"/>
-        <v>353</v>
+        <f>SUM(D15:L15)</f>
+        <v>458</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B16" s="5">
-        <v>4800</v>
+        <v>9999</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D16" s="6">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="E16" s="6">
+        <v>322</v>
+      </c>
+      <c r="F16" s="6">
+        <v>1</v>
+      </c>
+      <c r="G16" s="6">
+        <v>24</v>
+      </c>
+      <c r="H16" s="6">
+        <v>5</v>
+      </c>
+      <c r="I16" s="6">
+        <v>0</v>
+      </c>
+      <c r="J16" s="6">
+        <v>44</v>
+      </c>
+      <c r="K16" s="6">
+        <v>72</v>
+      </c>
+      <c r="L16" s="6">
+        <v>30</v>
+      </c>
+      <c r="M16" s="6">
+        <f>SUM(D16:L16)</f>
+        <v>520</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="G17" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="H17" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="I17" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="F16" s="6">
-        <v>0</v>
-      </c>
-      <c r="G16" s="6">
-        <v>0</v>
-      </c>
-      <c r="H16" s="6">
-        <v>0</v>
-      </c>
-      <c r="I16" s="6">
-        <v>0</v>
-      </c>
-      <c r="J16" s="6">
-        <v>0</v>
-      </c>
-      <c r="K16" s="6">
+      <c r="J17" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="K17" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="L17" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="M17" s="21" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="L16" s="6">
-        <v>1</v>
-      </c>
-      <c r="M16" s="6">
-        <f t="shared" si="2"/>
+      <c r="D18" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="F18" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="G18" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="H18" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="I18" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="J18" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="K18" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="L18" s="20" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17" s="9">
-        <v>9999</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17" s="10">
+      <c r="M18" s="20" t="s">
         <v>12</v>
-      </c>
-      <c r="E17" s="10">
-        <v>266</v>
-      </c>
-      <c r="F17" s="10">
-        <v>8</v>
-      </c>
-      <c r="G17" s="10">
-        <v>17</v>
-      </c>
-      <c r="H17" s="10">
-        <v>11</v>
-      </c>
-      <c r="I17" s="10">
-        <v>1</v>
-      </c>
-      <c r="J17" s="10">
-        <v>30</v>
-      </c>
-      <c r="K17" s="10">
-        <v>83</v>
-      </c>
-      <c r="L17" s="10">
-        <v>47</v>
-      </c>
-      <c r="M17" s="10">
-        <f t="shared" si="2"/>
-        <v>475</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" s="11"/>
-      <c r="C18" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D18" s="12">
-        <f t="shared" ref="D18:M18" si="3">SUM(D11:D17)</f>
-        <v>129</v>
-      </c>
-      <c r="E18" s="12">
-        <f t="shared" si="3"/>
-        <v>2237</v>
-      </c>
-      <c r="F18" s="12">
-        <f t="shared" si="3"/>
-        <v>36</v>
-      </c>
-      <c r="G18" s="12">
-        <f t="shared" si="3"/>
-        <v>192</v>
-      </c>
-      <c r="H18" s="12">
-        <f t="shared" si="3"/>
-        <v>76</v>
-      </c>
-      <c r="I18" s="12">
-        <f t="shared" si="3"/>
-        <v>4</v>
-      </c>
-      <c r="J18" s="12">
-        <f t="shared" si="3"/>
-        <v>164</v>
-      </c>
-      <c r="K18" s="12">
-        <f t="shared" si="3"/>
-        <v>706</v>
-      </c>
-      <c r="L18" s="12">
-        <f t="shared" si="3"/>
-        <v>311</v>
-      </c>
-      <c r="M18" s="12">
-        <f t="shared" si="3"/>
-        <v>3855</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1308,92 +1313,91 @@
       </c>
     </row>
     <row r="20" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20" s="5">
-        <v>860</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D20" s="6">
-        <v>0</v>
-      </c>
-      <c r="E20" s="6">
+      <c r="A20" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F20" s="6">
-        <v>0</v>
-      </c>
-      <c r="G20" s="6">
-        <v>0</v>
-      </c>
-      <c r="H20" s="6">
-        <v>0</v>
-      </c>
-      <c r="I20" s="6">
-        <v>0</v>
-      </c>
-      <c r="J20" s="6">
-        <v>0</v>
-      </c>
-      <c r="K20" s="6">
-        <v>0</v>
-      </c>
-      <c r="L20" s="6">
-        <v>1</v>
-      </c>
-      <c r="M20" s="6">
-        <f t="shared" ref="M20:M26" si="4">SUM(D20:L20)</f>
+      <c r="C20" s="3" t="s">
         <v>2</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L20" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M20" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="B21" s="5">
-        <v>1290</v>
+        <v>3830</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D21" s="6">
-        <v>123</v>
+        <v>0</v>
       </c>
       <c r="E21" s="6">
-        <v>1220</v>
+        <v>7</v>
       </c>
       <c r="F21" s="6">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="G21" s="6">
-        <v>103</v>
+        <v>0</v>
       </c>
       <c r="H21" s="6">
-        <v>56</v>
+        <v>0</v>
       </c>
       <c r="I21" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J21" s="6">
-        <v>130</v>
+        <v>1</v>
       </c>
       <c r="K21" s="6">
-        <v>491</v>
+        <v>1</v>
       </c>
       <c r="L21" s="6">
-        <v>262</v>
+        <v>0</v>
       </c>
       <c r="M21" s="6">
-        <f t="shared" si="4"/>
-        <v>2418</v>
+        <f>SUM(D21:L21)</f>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B22" s="5">
         <v>3830</v>
@@ -1405,32 +1409,32 @@
         <v>0</v>
       </c>
       <c r="E22" s="6">
+        <v>1</v>
+      </c>
+      <c r="F22" s="6">
+        <v>0</v>
+      </c>
+      <c r="G22" s="6">
+        <v>0</v>
+      </c>
+      <c r="H22" s="6">
+        <v>0</v>
+      </c>
+      <c r="I22" s="6">
+        <v>0</v>
+      </c>
+      <c r="J22" s="6">
+        <v>0</v>
+      </c>
+      <c r="K22" s="6">
         <v>3</v>
       </c>
-      <c r="F22" s="6">
-        <v>0</v>
-      </c>
-      <c r="G22" s="6">
+      <c r="L22" s="6">
         <v>1</v>
       </c>
-      <c r="H22" s="6">
-        <v>0</v>
-      </c>
-      <c r="I22" s="6">
-        <v>1</v>
-      </c>
-      <c r="J22" s="6">
-        <v>1</v>
-      </c>
-      <c r="K22" s="6">
-        <v>2</v>
-      </c>
-      <c r="L22" s="6">
-        <v>0</v>
-      </c>
       <c r="M22" s="6">
-        <f t="shared" si="4"/>
-        <v>8</v>
+        <f>SUM(D22:L22)</f>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1438,103 +1442,103 @@
         <v>22</v>
       </c>
       <c r="B23" s="5">
-        <v>4050</v>
+        <v>3830</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D23" s="6">
         <v>0</v>
       </c>
       <c r="E23" s="6">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F23" s="6">
         <v>0</v>
       </c>
       <c r="G23" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H23" s="6">
         <v>0</v>
       </c>
       <c r="I23" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J23" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K23" s="6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L23" s="6">
         <v>0</v>
       </c>
       <c r="M23" s="6">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f>SUM(D23:L23)</f>
+        <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B24" s="5">
-        <v>4260</v>
+        <v>3830</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D24" s="6">
+        <v>0</v>
+      </c>
+      <c r="E24" s="6">
         <v>3</v>
       </c>
-      <c r="E24" s="6">
-        <v>189</v>
-      </c>
       <c r="F24" s="6">
+        <v>0</v>
+      </c>
+      <c r="G24" s="6">
+        <v>0</v>
+      </c>
+      <c r="H24" s="6">
+        <v>0</v>
+      </c>
+      <c r="I24" s="6">
+        <v>0</v>
+      </c>
+      <c r="J24" s="6">
         <v>1</v>
       </c>
-      <c r="G24" s="6">
-        <v>7</v>
-      </c>
-      <c r="H24" s="6">
-        <v>8</v>
-      </c>
-      <c r="I24" s="6">
-        <v>0</v>
-      </c>
-      <c r="J24" s="6">
-        <v>9</v>
-      </c>
       <c r="K24" s="6">
-        <v>41</v>
+        <v>1</v>
       </c>
       <c r="L24" s="6">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="M24" s="6">
-        <f t="shared" si="4"/>
-        <v>305</v>
+        <f>SUM(D24:L24)</f>
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B25" s="5">
-        <v>4800</v>
+        <v>3830</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D25" s="6">
         <v>0</v>
       </c>
       <c r="E25" s="6">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F25" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G25" s="6">
         <v>0</v>
@@ -1552,143 +1556,137 @@
         <v>3</v>
       </c>
       <c r="L25" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M25" s="6">
-        <f t="shared" si="4"/>
-        <v>11</v>
+        <f>SUM(D25:L25)</f>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="8" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B26" s="9">
-        <v>9999</v>
+        <v>4050</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D26" s="10">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="E26" s="10">
-        <v>171</v>
+        <v>0</v>
       </c>
       <c r="F26" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G26" s="10">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="H26" s="10">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="I26" s="10">
         <v>0</v>
       </c>
       <c r="J26" s="10">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="K26" s="10">
-        <v>85</v>
+        <v>0</v>
       </c>
       <c r="L26" s="10">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="M26" s="10">
-        <f t="shared" si="4"/>
-        <v>342</v>
+        <f>SUM(D26:L26)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B27" s="11"/>
-      <c r="C27" s="11" t="s">
-        <v>12</v>
+      <c r="B27" s="14">
+        <v>4050</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>17</v>
       </c>
       <c r="D27" s="12">
-        <f t="shared" ref="D27:M27" si="5">SUM(D20:D26)</f>
-        <v>137</v>
+        <v>0</v>
       </c>
       <c r="E27" s="12">
-        <f t="shared" si="5"/>
-        <v>1589</v>
+        <v>0</v>
       </c>
       <c r="F27" s="12">
-        <f t="shared" si="5"/>
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="G27" s="12">
-        <f t="shared" si="5"/>
-        <v>122</v>
+        <v>0</v>
       </c>
       <c r="H27" s="12">
-        <f t="shared" si="5"/>
-        <v>69</v>
+        <v>0</v>
       </c>
       <c r="I27" s="12">
-        <f t="shared" si="5"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J27" s="12">
-        <f t="shared" si="5"/>
-        <v>163</v>
+        <v>0</v>
       </c>
       <c r="K27" s="12">
-        <f t="shared" si="5"/>
-        <v>622</v>
+        <v>0</v>
       </c>
       <c r="L27" s="12">
-        <f t="shared" si="5"/>
-        <v>347</v>
+        <v>0</v>
       </c>
       <c r="M27" s="12">
-        <f t="shared" si="5"/>
-        <v>3086</v>
+        <f>SUM(D27:L27)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H28" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I28" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J28" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K28" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="L28" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="M28" s="3" t="s">
-        <v>12</v>
+      <c r="A28" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B28" s="5">
+        <v>4050</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D28" s="6">
+        <v>0</v>
+      </c>
+      <c r="E28" s="6">
+        <v>0</v>
+      </c>
+      <c r="F28" s="6">
+        <v>0</v>
+      </c>
+      <c r="G28" s="6">
+        <v>0</v>
+      </c>
+      <c r="H28" s="6">
+        <v>0</v>
+      </c>
+      <c r="I28" s="6">
+        <v>0</v>
+      </c>
+      <c r="J28" s="6">
+        <v>0</v>
+      </c>
+      <c r="K28" s="6">
+        <v>0</v>
+      </c>
+      <c r="L28" s="6">
+        <v>0</v>
+      </c>
+      <c r="M28" s="6">
+        <f>SUM(D28:L28)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1696,22 +1694,22 @@
         <v>23</v>
       </c>
       <c r="B29" s="5">
-        <v>860</v>
+        <v>4050</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D29" s="6">
         <v>0</v>
       </c>
       <c r="E29" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F29" s="6">
         <v>0</v>
       </c>
       <c r="G29" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H29" s="6">
         <v>0</v>
@@ -1729,8 +1727,8 @@
         <v>0</v>
       </c>
       <c r="M29" s="6">
-        <f t="shared" ref="M29:M35" si="6">SUM(D29:L29)</f>
-        <v>2</v>
+        <f>SUM(D29:L29)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1738,130 +1736,130 @@
         <v>23</v>
       </c>
       <c r="B30" s="5">
-        <v>1290</v>
+        <v>4050</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D30" s="6">
-        <v>104</v>
+        <v>0</v>
       </c>
       <c r="E30" s="6">
-        <v>1409</v>
+        <v>3</v>
       </c>
       <c r="F30" s="6">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="G30" s="6">
-        <v>116</v>
+        <v>0</v>
       </c>
       <c r="H30" s="6">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="I30" s="6">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="J30" s="6">
-        <v>156</v>
+        <v>1</v>
       </c>
       <c r="K30" s="6">
-        <v>482</v>
+        <v>0</v>
       </c>
       <c r="L30" s="6">
-        <v>219</v>
+        <v>0</v>
       </c>
       <c r="M30" s="6">
-        <f t="shared" si="6"/>
-        <v>2520</v>
+        <f>SUM(D30:L30)</f>
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="B31" s="5">
-        <v>3830</v>
+        <v>4260</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D31" s="6">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E31" s="6">
+        <v>250</v>
+      </c>
+      <c r="F31" s="6">
+        <v>1</v>
+      </c>
+      <c r="G31" s="6">
+        <v>33</v>
+      </c>
+      <c r="H31" s="6">
         <v>3</v>
       </c>
-      <c r="F31" s="6">
-        <v>0</v>
-      </c>
-      <c r="G31" s="6">
-        <v>0</v>
-      </c>
-      <c r="H31" s="6">
-        <v>0</v>
-      </c>
       <c r="I31" s="6">
         <v>0</v>
       </c>
       <c r="J31" s="6">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="K31" s="6">
-        <v>1</v>
+        <v>62</v>
       </c>
       <c r="L31" s="6">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="M31" s="6">
-        <f t="shared" si="6"/>
-        <v>6</v>
+        <f>SUM(D31:L31)</f>
+        <v>414</v>
       </c>
     </row>
     <row r="32" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B32" s="5">
-        <v>4050</v>
+        <v>4260</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D32" s="6">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E32" s="6">
-        <v>0</v>
+        <v>244</v>
       </c>
       <c r="F32" s="6">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G32" s="6">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="H32" s="6">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="I32" s="6">
         <v>0</v>
       </c>
       <c r="J32" s="6">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K32" s="6">
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="L32" s="6">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="M32" s="6">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f>SUM(D32:L32)</f>
+        <v>353</v>
       </c>
     </row>
     <row r="33" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B33" s="5">
         <v>4260</v>
@@ -1870,35 +1868,35 @@
         <v>18</v>
       </c>
       <c r="D33" s="6">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E33" s="6">
-        <v>237</v>
+        <v>189</v>
       </c>
       <c r="F33" s="6">
         <v>1</v>
       </c>
       <c r="G33" s="6">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="H33" s="6">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="I33" s="6">
         <v>0</v>
       </c>
       <c r="J33" s="6">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="K33" s="6">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="L33" s="6">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="M33" s="6">
-        <f t="shared" si="6"/>
-        <v>330</v>
+        <f>SUM(D33:L33)</f>
+        <v>305</v>
       </c>
     </row>
     <row r="34" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1906,22 +1904,22 @@
         <v>23</v>
       </c>
       <c r="B34" s="5">
-        <v>4800</v>
+        <v>4260</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D34" s="6">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E34" s="6">
-        <v>6</v>
+        <v>237</v>
       </c>
       <c r="F34" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G34" s="6">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="H34" s="6">
         <v>0</v>
@@ -1930,17 +1928,17 @@
         <v>0</v>
       </c>
       <c r="J34" s="6">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="K34" s="6">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="L34" s="6">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="M34" s="6">
-        <f t="shared" si="6"/>
-        <v>10</v>
+        <f>SUM(D34:L34)</f>
+        <v>330</v>
       </c>
     </row>
     <row r="35" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1948,274 +1946,303 @@
         <v>23</v>
       </c>
       <c r="B35" s="9">
-        <v>9999</v>
+        <v>4260</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D35" s="10">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E35" s="10">
-        <v>259</v>
+        <v>235</v>
       </c>
       <c r="F35" s="10">
+        <v>0</v>
+      </c>
+      <c r="G35" s="10">
+        <v>19</v>
+      </c>
+      <c r="H35" s="10">
+        <v>5</v>
+      </c>
+      <c r="I35" s="10">
         <v>1</v>
       </c>
-      <c r="G35" s="10">
-        <v>14</v>
-      </c>
-      <c r="H35" s="10">
-        <v>6</v>
-      </c>
-      <c r="I35" s="10">
-        <v>0</v>
-      </c>
       <c r="J35" s="10">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="K35" s="10">
-        <v>98</v>
+        <v>41</v>
       </c>
       <c r="L35" s="10">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="M35" s="10">
-        <f t="shared" si="6"/>
-        <v>458</v>
+        <f>SUM(D35:L35)</f>
+        <v>338</v>
       </c>
     </row>
     <row r="36" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="11" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="B36" s="11"/>
       <c r="C36" s="11" t="s">
         <v>12</v>
       </c>
       <c r="D36" s="12">
-        <f t="shared" ref="D36:M36" si="7">SUM(D29:D35)</f>
-        <v>123</v>
+        <f>SUM(D29:D35)</f>
+        <v>35</v>
       </c>
       <c r="E36" s="12">
-        <f t="shared" si="7"/>
-        <v>1915</v>
+        <f>SUM(E29:E35)</f>
+        <v>1158</v>
       </c>
       <c r="F36" s="12">
-        <f t="shared" si="7"/>
-        <v>18</v>
+        <f>SUM(F29:F35)</f>
+        <v>6</v>
       </c>
       <c r="G36" s="12">
-        <f t="shared" si="7"/>
-        <v>145</v>
+        <f>SUM(G29:G35)</f>
+        <v>94</v>
       </c>
       <c r="H36" s="12">
-        <f t="shared" si="7"/>
-        <v>16</v>
+        <f>SUM(H29:H35)</f>
+        <v>23</v>
       </c>
       <c r="I36" s="12">
-        <f t="shared" si="7"/>
-        <v>8</v>
+        <f>SUM(I29:I35)</f>
+        <v>1</v>
       </c>
       <c r="J36" s="12">
-        <f t="shared" si="7"/>
-        <v>210</v>
+        <f>SUM(J29:J35)</f>
+        <v>44</v>
       </c>
       <c r="K36" s="12">
-        <f t="shared" si="7"/>
-        <v>619</v>
+        <f>SUM(K29:K35)</f>
+        <v>226</v>
       </c>
       <c r="L36" s="12">
-        <f t="shared" si="7"/>
-        <v>272</v>
+        <f>SUM(L29:L35)</f>
+        <v>157</v>
       </c>
       <c r="M36" s="12">
-        <f t="shared" si="7"/>
-        <v>3326</v>
+        <f>SUM(M29:M35)</f>
+        <v>1744</v>
       </c>
     </row>
     <row r="37" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C37" s="3" t="s">
+      <c r="A37" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D37" s="6">
+        <f>SUM(D30:D36)</f>
+        <v>70</v>
+      </c>
+      <c r="E37" s="6">
+        <f>SUM(E30:E36)</f>
+        <v>2316</v>
+      </c>
+      <c r="F37" s="6">
+        <f>SUM(F30:F36)</f>
+        <v>12</v>
+      </c>
+      <c r="G37" s="6">
+        <f>SUM(G30:G36)</f>
+        <v>188</v>
+      </c>
+      <c r="H37" s="6">
+        <f>SUM(H30:H36)</f>
+        <v>46</v>
+      </c>
+      <c r="I37" s="6">
+        <f>SUM(I30:I36)</f>
         <v>2</v>
       </c>
-      <c r="D37" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F37" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G37" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H37" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I37" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J37" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K37" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="L37" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="M37" s="3" t="s">
-        <v>12</v>
+      <c r="J37" s="6">
+        <f>SUM(J30:J36)</f>
+        <v>88</v>
+      </c>
+      <c r="K37" s="6">
+        <f>SUM(K30:K36)</f>
+        <v>452</v>
+      </c>
+      <c r="L37" s="6">
+        <f>SUM(L30:L36)</f>
+        <v>314</v>
+      </c>
+      <c r="M37" s="6">
+        <f>SUM(M30:M36)</f>
+        <v>3488</v>
       </c>
     </row>
     <row r="38" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B38" s="5">
-        <v>860</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>14</v>
+        <v>21</v>
+      </c>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="D38" s="6">
-        <v>0</v>
+        <f>SUM(D31:D37)</f>
+        <v>140</v>
       </c>
       <c r="E38" s="6">
-        <v>2</v>
+        <f>SUM(E31:E37)</f>
+        <v>4629</v>
       </c>
       <c r="F38" s="6">
-        <v>0</v>
+        <f>SUM(F31:F37)</f>
+        <v>24</v>
       </c>
       <c r="G38" s="6">
-        <v>1</v>
+        <f>SUM(G31:G37)</f>
+        <v>376</v>
       </c>
       <c r="H38" s="6">
-        <v>0</v>
+        <f>SUM(H31:H37)</f>
+        <v>92</v>
       </c>
       <c r="I38" s="6">
-        <v>0</v>
+        <f>SUM(I31:I37)</f>
+        <v>4</v>
       </c>
       <c r="J38" s="6">
-        <v>0</v>
+        <f>SUM(J31:J37)</f>
+        <v>175</v>
       </c>
       <c r="K38" s="6">
-        <v>1</v>
+        <f>SUM(K31:K37)</f>
+        <v>904</v>
       </c>
       <c r="L38" s="6">
-        <v>0</v>
+        <f>SUM(L31:L37)</f>
+        <v>628</v>
       </c>
       <c r="M38" s="6">
-        <f t="shared" ref="M38:M44" si="8">SUM(D38:L38)</f>
-        <v>4</v>
+        <f>SUM(M31:M37)</f>
+        <v>6972</v>
       </c>
     </row>
     <row r="39" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B39" s="5">
-        <v>1290</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>15</v>
+      <c r="B39" s="4"/>
+      <c r="C39" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="D39" s="6">
-        <v>97</v>
+        <f>SUM(D32:D38)</f>
+        <v>267</v>
       </c>
       <c r="E39" s="6">
-        <v>1597</v>
+        <f>SUM(E32:E38)</f>
+        <v>9008</v>
       </c>
       <c r="F39" s="6">
-        <v>5</v>
+        <f>SUM(F32:F38)</f>
+        <v>47</v>
       </c>
       <c r="G39" s="6">
-        <v>123</v>
+        <f>SUM(G32:G38)</f>
+        <v>719</v>
       </c>
       <c r="H39" s="6">
-        <v>22</v>
+        <f>SUM(H32:H38)</f>
+        <v>181</v>
       </c>
       <c r="I39" s="6">
-        <v>11</v>
+        <f>SUM(I32:I38)</f>
+        <v>8</v>
       </c>
       <c r="J39" s="6">
-        <v>149</v>
+        <f>SUM(J32:J38)</f>
+        <v>338</v>
       </c>
       <c r="K39" s="6">
-        <v>489</v>
+        <f>SUM(K32:K38)</f>
+        <v>1746</v>
       </c>
       <c r="L39" s="6">
-        <v>187</v>
+        <f>SUM(L32:L38)</f>
+        <v>1216</v>
       </c>
       <c r="M39" s="6">
-        <f t="shared" si="8"/>
-        <v>2680</v>
+        <f>SUM(M32:M38)</f>
+        <v>13530</v>
       </c>
     </row>
     <row r="40" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B40" s="5">
-        <v>3830</v>
-      </c>
-      <c r="C40" s="5" t="s">
+      <c r="B40" s="4"/>
+      <c r="C40" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D40" s="6">
+        <f>SUM(D33:D39)</f>
+        <v>528</v>
+      </c>
+      <c r="E40" s="6">
+        <f>SUM(E33:E39)</f>
+        <v>17772</v>
+      </c>
+      <c r="F40" s="6">
+        <f>SUM(F33:F39)</f>
+        <v>91</v>
+      </c>
+      <c r="G40" s="6">
+        <f>SUM(G33:G39)</f>
+        <v>1417</v>
+      </c>
+      <c r="H40" s="6">
+        <f>SUM(H33:H39)</f>
+        <v>355</v>
+      </c>
+      <c r="I40" s="6">
+        <f>SUM(I33:I39)</f>
         <v>16</v>
       </c>
-      <c r="D40" s="6">
-        <v>0</v>
-      </c>
-      <c r="E40" s="6">
-        <v>1</v>
-      </c>
-      <c r="F40" s="6">
-        <v>0</v>
-      </c>
-      <c r="G40" s="6">
-        <v>0</v>
-      </c>
-      <c r="H40" s="6">
-        <v>0</v>
-      </c>
-      <c r="I40" s="6">
-        <v>0</v>
-      </c>
       <c r="J40" s="6">
-        <v>1</v>
+        <f>SUM(J33:J39)</f>
+        <v>671</v>
       </c>
       <c r="K40" s="6">
-        <v>3</v>
+        <f>SUM(K33:K39)</f>
+        <v>3445</v>
       </c>
       <c r="L40" s="6">
-        <v>0</v>
+        <f>SUM(L33:L39)</f>
+        <v>2412</v>
       </c>
       <c r="M40" s="6">
-        <f t="shared" si="8"/>
-        <v>5</v>
+        <f>SUM(M33:M39)</f>
+        <v>26707</v>
       </c>
     </row>
     <row r="41" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="B41" s="5">
-        <v>4050</v>
+        <v>4800</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D41" s="6">
         <v>0</v>
       </c>
       <c r="E41" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F41" s="6">
         <v>0</v>
@@ -2230,64 +2257,64 @@
         <v>0</v>
       </c>
       <c r="J41" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K41" s="6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L41" s="6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M41" s="6">
-        <f t="shared" si="8"/>
-        <v>4</v>
+        <f>SUM(D41:L41)</f>
+        <v>8</v>
       </c>
     </row>
     <row r="42" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B42" s="5">
-        <v>4260</v>
+        <v>4800</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D42" s="6">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E42" s="6">
-        <v>235</v>
+        <v>8</v>
       </c>
       <c r="F42" s="6">
         <v>0</v>
       </c>
       <c r="G42" s="6">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="H42" s="6">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="I42" s="6">
+        <v>0</v>
+      </c>
+      <c r="J42" s="6">
+        <v>0</v>
+      </c>
+      <c r="K42" s="6">
+        <v>2</v>
+      </c>
+      <c r="L42" s="6">
         <v>1</v>
       </c>
-      <c r="J42" s="6">
-        <v>10</v>
-      </c>
-      <c r="K42" s="6">
-        <v>41</v>
-      </c>
-      <c r="L42" s="6">
-        <v>22</v>
-      </c>
       <c r="M42" s="6">
-        <f t="shared" si="8"/>
-        <v>338</v>
+        <f>SUM(D42:L42)</f>
+        <v>11</v>
       </c>
     </row>
     <row r="43" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B43" s="5">
         <v>4800</v>
@@ -2299,10 +2326,10 @@
         <v>0</v>
       </c>
       <c r="E43" s="6">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F43" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G43" s="6">
         <v>0</v>
@@ -2314,16 +2341,16 @@
         <v>0</v>
       </c>
       <c r="J43" s="6">
+        <v>1</v>
+      </c>
+      <c r="K43" s="6">
         <v>3</v>
       </c>
-      <c r="K43" s="6">
-        <v>2</v>
-      </c>
       <c r="L43" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M43" s="6">
-        <f t="shared" si="8"/>
+        <f>SUM(D43:L43)</f>
         <v>11</v>
       </c>
     </row>
@@ -2332,143 +2359,166 @@
         <v>23</v>
       </c>
       <c r="B44" s="9">
-        <v>9999</v>
+        <v>4800</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D44" s="10">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="E44" s="10">
-        <v>322</v>
+        <v>6</v>
       </c>
       <c r="F44" s="10">
+        <v>0</v>
+      </c>
+      <c r="G44" s="10">
+        <v>0</v>
+      </c>
+      <c r="H44" s="10">
+        <v>0</v>
+      </c>
+      <c r="I44" s="10">
+        <v>0</v>
+      </c>
+      <c r="J44" s="10">
         <v>1</v>
       </c>
-      <c r="G44" s="10">
-        <v>24</v>
-      </c>
-      <c r="H44" s="10">
-        <v>5</v>
-      </c>
-      <c r="I44" s="10">
-        <v>0</v>
-      </c>
-      <c r="J44" s="10">
-        <v>44</v>
-      </c>
       <c r="K44" s="10">
-        <v>72</v>
+        <v>3</v>
       </c>
       <c r="L44" s="10">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="M44" s="10">
-        <f t="shared" si="8"/>
-        <v>520</v>
+        <f>SUM(D44:L44)</f>
+        <v>10</v>
       </c>
     </row>
     <row r="45" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B45" s="11"/>
-      <c r="C45" s="11" t="s">
+      <c r="B45" s="14">
+        <v>4800</v>
+      </c>
+      <c r="C45" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D45" s="12">
+        <v>0</v>
+      </c>
+      <c r="E45" s="12">
+        <v>6</v>
+      </c>
+      <c r="F45" s="12">
+        <v>0</v>
+      </c>
+      <c r="G45" s="12">
+        <v>0</v>
+      </c>
+      <c r="H45" s="12">
+        <v>0</v>
+      </c>
+      <c r="I45" s="12">
+        <v>0</v>
+      </c>
+      <c r="J45" s="12">
+        <v>3</v>
+      </c>
+      <c r="K45" s="12">
+        <v>2</v>
+      </c>
+      <c r="L45" s="12">
+        <v>0</v>
+      </c>
+      <c r="M45" s="12">
+        <f>SUM(D45:L45)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H46" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I46" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J46" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K46" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L46" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M46" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D45" s="12">
-        <f t="shared" ref="D45:M45" si="9">SUM(D38:D44)</f>
-        <v>124</v>
-      </c>
-      <c r="E45" s="12">
-        <f t="shared" si="9"/>
-        <v>2166</v>
-      </c>
-      <c r="F45" s="12">
-        <f t="shared" si="9"/>
-        <v>6</v>
-      </c>
-      <c r="G45" s="12">
-        <f t="shared" si="9"/>
-        <v>167</v>
-      </c>
-      <c r="H45" s="12">
-        <f t="shared" si="9"/>
-        <v>32</v>
-      </c>
-      <c r="I45" s="12">
-        <f t="shared" si="9"/>
-        <v>12</v>
-      </c>
-      <c r="J45" s="12">
-        <f t="shared" si="9"/>
-        <v>208</v>
-      </c>
-      <c r="K45" s="12">
-        <f t="shared" si="9"/>
-        <v>608</v>
-      </c>
-      <c r="L45" s="12">
-        <f t="shared" si="9"/>
-        <v>239</v>
-      </c>
-      <c r="M45" s="12">
-        <f t="shared" si="9"/>
-        <v>3562</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
-      <c r="F46" s="1"/>
-      <c r="G46" s="1"/>
-      <c r="H46" s="1"/>
-      <c r="I46" s="1"/>
-      <c r="J46" s="1"/>
-      <c r="K46" s="1"/>
-      <c r="L46" s="1"/>
-      <c r="M46" s="1"/>
     </row>
     <row r="47" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C47" s="3" t="s">
+      <c r="A47" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B47" s="5">
+        <v>860</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D47" s="6">
+        <v>0</v>
+      </c>
+      <c r="E47" s="6">
+        <v>3</v>
+      </c>
+      <c r="F47" s="6">
+        <v>0</v>
+      </c>
+      <c r="G47" s="6">
+        <v>0</v>
+      </c>
+      <c r="H47" s="6">
+        <v>0</v>
+      </c>
+      <c r="I47" s="6">
+        <v>0</v>
+      </c>
+      <c r="J47" s="6">
         <v>2</v>
       </c>
-      <c r="D47" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E47" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F47" s="3" t="s">
+      <c r="K47" s="6">
+        <v>0</v>
+      </c>
+      <c r="L47" s="6">
+        <v>0</v>
+      </c>
+      <c r="M47" s="6">
+        <f>SUM(D47:L47)</f>
         <v>5</v>
-      </c>
-      <c r="G47" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H47" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I47" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J47" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K47" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="L47" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="M47" s="3" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="48" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2476,41 +2526,41 @@
         <v>24</v>
       </c>
       <c r="B48" s="5">
-        <v>860</v>
+        <v>1290</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D48" s="6">
-        <v>0</v>
+        <v>154</v>
       </c>
       <c r="E48" s="6">
-        <v>3</v>
+        <v>1708</v>
       </c>
       <c r="F48" s="6">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="G48" s="6">
-        <v>0</v>
+        <v>181</v>
       </c>
       <c r="H48" s="6">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="I48" s="6">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="J48" s="6">
-        <v>2</v>
+        <v>144</v>
       </c>
       <c r="K48" s="6">
-        <v>0</v>
+        <v>591</v>
       </c>
       <c r="L48" s="6">
-        <v>0</v>
+        <v>179</v>
       </c>
       <c r="M48" s="6">
-        <f t="shared" ref="M48:M54" si="10">SUM(D48:L48)</f>
-        <v>5</v>
+        <f>SUM(D48:L48)</f>
+        <v>3003</v>
       </c>
     </row>
     <row r="49" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2518,41 +2568,41 @@
         <v>24</v>
       </c>
       <c r="B49" s="5">
-        <v>1290</v>
+        <v>3830</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D49" s="6">
-        <v>154</v>
+        <v>0</v>
       </c>
       <c r="E49" s="6">
-        <v>1708</v>
+        <v>1</v>
       </c>
       <c r="F49" s="6">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="G49" s="6">
-        <v>181</v>
+        <v>0</v>
       </c>
       <c r="H49" s="6">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="I49" s="6">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="J49" s="6">
-        <v>144</v>
+        <v>1</v>
       </c>
       <c r="K49" s="6">
-        <v>591</v>
+        <v>0</v>
       </c>
       <c r="L49" s="6">
-        <v>179</v>
+        <v>0</v>
       </c>
       <c r="M49" s="6">
-        <f t="shared" si="10"/>
-        <v>3003</v>
+        <f>SUM(D49:L49)</f>
+        <v>2</v>
       </c>
     </row>
     <row r="50" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2560,10 +2610,10 @@
         <v>24</v>
       </c>
       <c r="B50" s="5">
-        <v>3830</v>
+        <v>4050</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D50" s="6">
         <v>0</v>
@@ -2584,7 +2634,7 @@
         <v>0</v>
       </c>
       <c r="J50" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K50" s="6">
         <v>0</v>
@@ -2593,8 +2643,8 @@
         <v>0</v>
       </c>
       <c r="M50" s="6">
-        <f t="shared" si="10"/>
-        <v>2</v>
+        <f>SUM(D50:L50)</f>
+        <v>3</v>
       </c>
     </row>
     <row r="51" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2602,41 +2652,41 @@
         <v>24</v>
       </c>
       <c r="B51" s="5">
-        <v>4050</v>
+        <v>4260</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D51" s="6">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E51" s="6">
-        <v>1</v>
+        <v>233</v>
       </c>
       <c r="F51" s="6">
         <v>0</v>
       </c>
       <c r="G51" s="6">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H51" s="6">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I51" s="6">
         <v>0</v>
       </c>
       <c r="J51" s="6">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="K51" s="6">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="L51" s="6">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="M51" s="6">
-        <f t="shared" si="10"/>
-        <v>3</v>
+        <f>SUM(D51:L51)</f>
+        <v>328</v>
       </c>
     </row>
     <row r="52" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2644,192 +2694,164 @@
         <v>24</v>
       </c>
       <c r="B52" s="5">
-        <v>4260</v>
+        <v>4800</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D52" s="6">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E52" s="6">
-        <v>233</v>
+        <v>12</v>
       </c>
       <c r="F52" s="6">
         <v>0</v>
       </c>
       <c r="G52" s="6">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="H52" s="6">
+        <v>0</v>
+      </c>
+      <c r="I52" s="6">
+        <v>0</v>
+      </c>
+      <c r="J52" s="6">
+        <v>1</v>
+      </c>
+      <c r="K52" s="6">
         <v>3</v>
       </c>
-      <c r="I52" s="6">
-        <v>0</v>
-      </c>
-      <c r="J52" s="6">
-        <v>10</v>
-      </c>
-      <c r="K52" s="6">
-        <v>40</v>
-      </c>
       <c r="L52" s="6">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="M52" s="6">
-        <f t="shared" si="10"/>
-        <v>328</v>
+        <f>SUM(D52:L52)</f>
+        <v>16</v>
       </c>
     </row>
     <row r="53" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="4" t="s">
+      <c r="A53" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B53" s="5">
-        <v>4800</v>
-      </c>
-      <c r="C53" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D53" s="6">
-        <v>0</v>
-      </c>
-      <c r="E53" s="6">
+      <c r="B53" s="9">
+        <v>9999</v>
+      </c>
+      <c r="C53" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D53" s="10">
+        <v>21</v>
+      </c>
+      <c r="E53" s="10">
+        <v>300</v>
+      </c>
+      <c r="F53" s="10">
+        <v>3</v>
+      </c>
+      <c r="G53" s="10">
+        <v>31</v>
+      </c>
+      <c r="H53" s="10">
+        <v>6</v>
+      </c>
+      <c r="I53" s="10">
+        <v>0</v>
+      </c>
+      <c r="J53" s="10">
+        <v>30</v>
+      </c>
+      <c r="K53" s="10">
+        <v>89</v>
+      </c>
+      <c r="L53" s="10">
+        <v>24</v>
+      </c>
+      <c r="M53" s="10">
+        <f>SUM(D53:L53)</f>
+        <v>504</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B54" s="11"/>
+      <c r="C54" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F53" s="6">
-        <v>0</v>
-      </c>
-      <c r="G53" s="6">
-        <v>0</v>
-      </c>
-      <c r="H53" s="6">
-        <v>0</v>
-      </c>
-      <c r="I53" s="6">
-        <v>0</v>
-      </c>
-      <c r="J53" s="6">
-        <v>1</v>
-      </c>
-      <c r="K53" s="6">
-        <v>3</v>
-      </c>
-      <c r="L53" s="6">
-        <v>0</v>
-      </c>
-      <c r="M53" s="6">
-        <f t="shared" si="10"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="54" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B54" s="9">
-        <v>9999</v>
-      </c>
-      <c r="C54" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D54" s="10">
-        <v>21</v>
-      </c>
-      <c r="E54" s="10">
-        <v>300</v>
-      </c>
-      <c r="F54" s="10">
-        <v>3</v>
-      </c>
-      <c r="G54" s="10">
-        <v>31</v>
-      </c>
-      <c r="H54" s="10">
-        <v>6</v>
-      </c>
-      <c r="I54" s="10">
-        <v>0</v>
-      </c>
-      <c r="J54" s="10">
-        <v>30</v>
-      </c>
-      <c r="K54" s="10">
-        <v>89</v>
-      </c>
-      <c r="L54" s="10">
-        <v>24</v>
-      </c>
-      <c r="M54" s="10">
-        <f t="shared" si="10"/>
-        <v>504</v>
+      <c r="D54" s="12">
+        <f>SUM(D47:D53)</f>
+        <v>182</v>
+      </c>
+      <c r="E54" s="12">
+        <f>SUM(E47:E53)</f>
+        <v>2258</v>
+      </c>
+      <c r="F54" s="12">
+        <f>SUM(F47:F53)</f>
+        <v>14</v>
+      </c>
+      <c r="G54" s="12">
+        <f>SUM(G47:G53)</f>
+        <v>220</v>
+      </c>
+      <c r="H54" s="12">
+        <f>SUM(H47:H53)</f>
+        <v>35</v>
+      </c>
+      <c r="I54" s="12">
+        <f>SUM(I47:I53)</f>
+        <v>9</v>
+      </c>
+      <c r="J54" s="12">
+        <f>SUM(J47:J53)</f>
+        <v>190</v>
+      </c>
+      <c r="K54" s="12">
+        <f>SUM(K47:K53)</f>
+        <v>723</v>
+      </c>
+      <c r="L54" s="12">
+        <f>SUM(L47:L53)</f>
+        <v>230</v>
+      </c>
+      <c r="M54" s="12">
+        <f>SUM(M47:M53)</f>
+        <v>3861</v>
       </c>
     </row>
     <row r="55" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="B55" s="11"/>
-      <c r="C55" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D55" s="12">
-        <f t="shared" ref="D55:M55" si="11">SUM(D48:D54)</f>
-        <v>182</v>
-      </c>
-      <c r="E55" s="12">
-        <f t="shared" si="11"/>
-        <v>2258</v>
-      </c>
-      <c r="F55" s="12">
-        <f t="shared" si="11"/>
-        <v>14</v>
-      </c>
-      <c r="G55" s="12">
-        <f t="shared" si="11"/>
-        <v>220</v>
-      </c>
-      <c r="H55" s="12">
-        <f t="shared" si="11"/>
-        <v>35</v>
-      </c>
-      <c r="I55" s="12">
-        <f t="shared" si="11"/>
-        <v>9</v>
-      </c>
-      <c r="J55" s="12">
-        <f t="shared" si="11"/>
-        <v>190</v>
-      </c>
-      <c r="K55" s="12">
-        <f t="shared" si="11"/>
-        <v>723</v>
-      </c>
-      <c r="L55" s="12">
-        <f t="shared" si="11"/>
-        <v>230</v>
-      </c>
-      <c r="M55" s="12">
-        <f t="shared" si="11"/>
-        <v>3861</v>
-      </c>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+      <c r="F55" s="1"/>
+      <c r="G55" s="1"/>
+      <c r="H55" s="1"/>
+      <c r="I55" s="1"/>
+      <c r="J55" s="1"/>
+      <c r="K55" s="1"/>
+      <c r="L55" s="1"/>
+      <c r="M55" s="1"/>
     </row>
     <row r="56" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D56" s="1"/>
-      <c r="E56" s="1"/>
-      <c r="F56" s="1"/>
-      <c r="G56" s="1"/>
-      <c r="H56" s="1"/>
-      <c r="I56" s="1"/>
-      <c r="J56" s="1"/>
-      <c r="K56" s="1"/>
-      <c r="L56" s="1"/>
-      <c r="M56" s="1"/>
+      <c r="A56" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B56" s="17"/>
+      <c r="C56" s="17"/>
+      <c r="D56" s="15"/>
+      <c r="E56" s="15"/>
+      <c r="F56" s="15"/>
+      <c r="G56" s="15"/>
+      <c r="H56" s="15"/>
+      <c r="I56" s="15"/>
+      <c r="J56" s="15"/>
+      <c r="K56" s="15"/>
+      <c r="L56" s="15"/>
+      <c r="M56" s="15"/>
     </row>
     <row r="57" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="7" t="s">
-        <v>25</v>
-      </c>
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
       <c r="F57" s="1"/>
@@ -14049,19 +14071,11 @@
       <c r="L991" s="1"/>
       <c r="M991" s="1"/>
     </row>
-    <row r="992" spans="4:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D992" s="1"/>
-      <c r="E992" s="1"/>
-      <c r="F992" s="1"/>
-      <c r="G992" s="1"/>
-      <c r="H992" s="1"/>
-      <c r="I992" s="1"/>
-      <c r="J992" s="1"/>
-      <c r="K992" s="1"/>
-      <c r="L992" s="1"/>
-      <c r="M992" s="1"/>
-    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M45">
+    <sortCondition ref="C2:C45"/>
+    <sortCondition ref="A2:A45"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
 </worksheet>

</xml_diff>